<commit_message>
STU3 corrections on AllergyIntolerance and Instance
</commit_message>
<xml_diff>
--- a/Mappings/AllergyIntolerantie - STU3.xlsx
+++ b/Mappings/AllergyIntolerantie - STU3.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -125,9 +125,6 @@
     <t>Notes/Issues</t>
   </si>
   <si>
-    <t>Have to add an extension</t>
-  </si>
-  <si>
     <t>Terminology mapt exact.</t>
   </si>
   <si>
@@ -320,19 +317,10 @@
     <t>Terminologie issue: FHIR Required VS binding:</t>
   </si>
   <si>
-    <t>AllergyIntolerance.clinicalStatus.extension</t>
-  </si>
-  <si>
-    <t>AllergyIntolerance.category.extension</t>
-  </si>
-  <si>
     <t>Terminologie issue: FHIR Required VS binding (gForge issue #10262: Biologic was added to the ValueSet per STU3)</t>
   </si>
   <si>
     <t>AllergyIntolerance.onset[x]</t>
-  </si>
-  <si>
-    <t>AllergyIntolerance.criticality.extension</t>
   </si>
   <si>
     <t>AllergyIntolerance.lastOccurence</t>
@@ -385,7 +373,64 @@
     <t>Terminology issue: in STU3 this element has become an extenstion. However, the valueset binding is still required en does not map with the ZIB valueset. (Gforge ID:10369)</t>
   </si>
   <si>
-    <t>AllergyIntolerance.reaction.extension.zib-allergyintolerance-certainty</t>
+    <t>Have to add an extension / FHIR core extension: http://hl7.org/fhir/extension-allergyintolerance-duration.html</t>
+  </si>
+  <si>
+    <r>
+      <t>AllergyIntolerance.reaction.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF484A4C"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>.zib-allergyintolerance-certainty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AllergyIntolerance.criticality.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>extension</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AllergyIntolerance.category.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>extension</t>
+    </r>
+  </si>
+  <si>
+    <t>AllergyIntolerance.clinicalStatus</t>
+  </si>
+  <si>
+    <t>Terminologie mapt… ZIB value 'Nullified' can be used in mandatory verificationStatus element</t>
+  </si>
+  <si>
+    <t>Terminology mapt exact. - Use  FHIR. Conceptmapping maken.</t>
   </si>
 </sst>
 </file>
@@ -775,36 +820,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1112,7 +1157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1122,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1139,15 +1184,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1160,16 +1205,16 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="3"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
       <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1180,10 +1225,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="45"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -1192,10 +1237,10 @@
         <v>5</v>
       </c>
       <c r="J3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="25.5">
@@ -1203,10 +1248,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -1215,21 +1260,21 @@
         <v>5</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="25.5">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -1238,10 +1283,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1249,10 +1294,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1261,7 +1306,7 @@
         <v>9</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1269,10 +1314,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1281,10 +1326,10 @@
         <v>11</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1292,10 +1337,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1304,7 +1349,7 @@
         <v>9</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K8" s="14"/>
     </row>
@@ -1313,10 +1358,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1325,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K9" s="14"/>
     </row>
@@ -1334,10 +1379,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1363,10 +1408,10 @@
         <v>11</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1386,10 +1431,10 @@
         <v>11</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="38.25">
@@ -1409,10 +1454,10 @@
         <v>5</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K13" s="28" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1432,7 +1477,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K14" s="14"/>
     </row>
@@ -1453,10 +1498,10 @@
         <v>5</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1476,10 +1521,10 @@
         <v>5</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1499,11 +1544,11 @@
         <v>9</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="25.5">
       <c r="A18" s="18">
         <v>16</v>
       </c>
@@ -1520,10 +1565,10 @@
         <v>25</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K18" s="27" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1594,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B16" sqref="A15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1563,93 +1608,93 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="C1" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="C2" s="31"/>
       <c r="D2" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="31"/>
       <c r="D3" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50.25" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="50.25" customHeight="1">
       <c r="A5" s="32"/>
       <c r="D5" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60.75" customHeight="1">
       <c r="A6" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="76.5" customHeight="1">
       <c r="A7" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1662,7 +1707,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1674,70 +1719,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="42"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="45"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1764,78 +1809,78 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="C1" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="77.25" customHeight="1">
       <c r="A3" s="30"/>
       <c r="D3" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="64.5" customHeight="1">
       <c r="A4" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="64.5" customHeight="1">
       <c r="A5" s="32"/>
       <c r="D5" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30.75" customHeight="1">
       <c r="A6" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>